<commit_message>
Global refactoring of the RestApi
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/Resource/environment.xlsx
+++ b/TestAutomationFramework/Resource/environment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\JuiceBoxQA\TestAutomationFramework\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Alpha</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>juiceboxdev.cloudapp.net</t>
+  </si>
+  <si>
+    <t>Stage</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -277,6 +280,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -557,20 +563,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.36328125" style="1" customWidth="1"/>
     <col min="2" max="4" width="54.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="29.26953125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -583,8 +590,11 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -598,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -612,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>

</xml_diff>